<commit_message>
Poprawka metody parującej adresy poztycji z L i P strony
</commit_message>
<xml_diff>
--- a/ExcelPln2/Input/BAT__VALID.xlsx
+++ b/ExcelPln2/Input/BAT__VALID.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>2 x Vogue Bleue Clic 812</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>4x9</t>
+  </si>
+  <si>
+    <t>aaa</t>
   </si>
 </sst>
 </file>
@@ -966,6 +969,24 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1011,24 +1032,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="=D:\WINNT\SYSTEM32\COMMAND.COM" xfId="4"/>
@@ -8126,53 +8129,121 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>224483</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>295848</xdr:rowOff>
+      <xdr:colOff>215137</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>96966</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>786458</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1257873</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="108" name="Picture 94"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="851859" y="1331017"/>
-          <a:ext cx="561975" cy="962025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="4F81BD"/>
+      <xdr:colOff>824737</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>982791</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Obraz 95"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="842513" y="1132135"/>
+          <a:ext cx="609600" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>230821</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1038030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>840421</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1923855</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="109" name="Obraz 95"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="858197" y="2073199"/>
+          <a:ext cx="609600" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
@@ -30324,7 +30395,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -30382,7 +30453,9 @@
       <c r="A5" s="52">
         <v>1</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
@@ -30968,16 +31041,16 @@
   <sheetData>
     <row r="1" spans="1:28" ht="14.95" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="72"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="74"/>
+      <c r="D3" s="80"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B4" s="55">
@@ -31292,10 +31365,10 @@
       <c r="S7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="T7" s="84" t="s">
+      <c r="T7" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="U7" s="85"/>
+      <c r="U7" s="70"/>
       <c r="V7" s="3" t="s">
         <v>45</v>
       </c>
@@ -31335,8 +31408,8 @@
       <c r="F8" s="13"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="87"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="72"/>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
@@ -31365,8 +31438,8 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="87"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="72"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="14"/>
@@ -31397,8 +31470,8 @@
       <c r="D10" s="16"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="87"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="72"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
       <c r="K10" s="18"/>
@@ -31429,8 +31502,8 @@
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="22"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="89"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="74"/>
       <c r="I11" s="22"/>
       <c r="J11" s="21"/>
       <c r="K11" s="23"/>
@@ -31461,8 +31534,8 @@
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
       <c r="F12" s="26"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="76"/>
       <c r="I12" s="25"/>
       <c r="J12" s="27"/>
       <c r="K12" s="25"/>
@@ -31493,8 +31566,8 @@
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
       <c r="I13" s="25"/>
       <c r="J13" s="25"/>
       <c r="K13" s="25"/>
@@ -31547,19 +31620,19 @@
     </row>
     <row r="15" spans="1:28" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="82" t="s">
         <v>55</v>
       </c>
       <c r="C15" s="33"/>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="84" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="33"/>
-      <c r="F15" s="80" t="s">
+      <c r="F15" s="86" t="s">
         <v>57</v>
       </c>
       <c r="G15" s="34"/>
-      <c r="H15" s="82" t="s">
+      <c r="H15" s="88" t="s">
         <v>58</v>
       </c>
       <c r="J15" s="33"/>
@@ -31582,18 +31655,13 @@
       <c r="AA15" s="33"/>
     </row>
     <row r="16" spans="1:28" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="77"/>
-      <c r="D16" s="79"/>
-      <c r="F16" s="81"/>
-      <c r="H16" s="83"/>
+      <c r="B16" s="83"/>
+      <c r="D16" s="85"/>
+      <c r="F16" s="87"/>
+      <c r="H16" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="T7:U7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
@@ -31602,6 +31670,11 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="H15:H16"/>
+    <mergeCell ref="T7:U7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>